<commit_message>
In 4_plots_or_ORRACE_average.qmd, made a corrplot of Oregon race and exit categories with standarized residuals
</commit_message>
<xml_diff>
--- a/Data/dq_odds_ratio_ci_table.xlsx
+++ b/Data/dq_odds_ratio_ci_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hata/Desktop/EDLD652_Diss/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F6E286-58D7-DA4A-9D42-C7766E284901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9AE48C-9C41-F846-95BE-F4CA08DB3BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18840" yWindow="660" windowWidth="13000" windowHeight="15680" activeTab="2" xr2:uid="{C07F39D0-090F-B744-8309-4E77EA4D3FDD}"/>
+    <workbookView xWindow="12520" yWindow="500" windowWidth="17360" windowHeight="15940" activeTab="2" xr2:uid="{C07F39D0-090F-B744-8309-4E77EA4D3FDD}"/>
   </bookViews>
   <sheets>
     <sheet name="race_us_vs_average" sheetId="1" r:id="rId1"/>
@@ -661,7 +661,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>